<commit_message>
add support for deductible with min and max (rule 26)
</commit_message>
<xml_diff>
--- a/oasislmf/_data/calc_rules.xlsx
+++ b/oasislmf/_data/calc_rules.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\OasisLMF\oasislmf\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\OasisLMF\oasislmf\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54147F6C-42A9-452D-AE90-8770D5D5BCEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC09781-1318-404B-957C-995C4E1E58F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calc_rules" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">calc_rules!$A$1:$M$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">calc_rules!$A$1:$M$83</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>desc</t>
   </si>
@@ -318,6 +318,15 @@
   </si>
   <si>
     <t>deductible with max. deductible; no limit % TIV</t>
+  </si>
+  <si>
+    <t>deductible with min and max deductible, no limit % loss</t>
+  </si>
+  <si>
+    <t>deductible with min and max deductible, no limit % TIV</t>
+  </si>
+  <si>
+    <t>deductible with min and max deductible, no limit</t>
   </si>
 </sst>
 </file>
@@ -1158,41 +1167,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M83"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A81" sqref="A81:M83"/>
+      <selection pane="bottomRight" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1233,7 +1242,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1275,7 +1284,7 @@
         <v>(1, 0, 0, 1, 0, 0, 0, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1317,7 +1326,7 @@
         <v>(1, 0, 0, 1, 1, 1, 0, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1359,7 +1368,7 @@
         <v>(1, 0, 0, 1, 0, 0, 0, 2, 0, 0)</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1401,7 +1410,7 @@
         <v>(1, 0, 0, 1, 0, 0, 2, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1443,7 +1452,7 @@
         <v>(1, 0, 0, 1, 0, 0, 1, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1485,7 +1494,7 @@
         <v>(1, 0, 0, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1527,7 +1536,7 @@
         <v>(1, 0, 0, 0, 0, 0, 2, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1569,7 +1578,7 @@
         <v>(1, 0, 0, 0, 0, 0, 2, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1611,7 +1620,7 @@
         <v>(0, 0, 1, 1, 0, 0, 0, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1653,7 +1662,7 @@
         <v>(0, 0, 1, 1, 0, 0, 1, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1695,7 +1704,7 @@
         <v>(0, 0, 1, 1, 0, 0, 2, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1737,7 +1746,7 @@
         <v>(0, 1, 0, 1, 0, 0, 0, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1779,7 +1788,7 @@
         <v>(0, 1, 0, 1, 0, 0, 1, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1821,7 +1830,7 @@
         <v>(0, 1, 0, 1, 0, 0, 2, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1863,7 +1872,7 @@
         <v>(1, 0, 0, 1, 0, 0, 2, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1905,7 +1914,7 @@
         <v>(0, 0, 1, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1947,7 +1956,7 @@
         <v>(0, 0, 1, 0, 0, 0, 0, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1989,7 +1998,7 @@
         <v>(0, 0, 1, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -2031,7 +2040,7 @@
         <v>(0, 0, 1, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -2073,7 +2082,7 @@
         <v>(0, 0, 1, 0, 0, 0, 1, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -2115,7 +2124,7 @@
         <v>(0, 0, 1, 0, 0, 0, 1, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2157,7 +2166,7 @@
         <v>(0, 0, 1, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -2199,7 +2208,7 @@
         <v>(0, 0, 1, 0, 0, 0, 2, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -2241,7 +2250,7 @@
         <v>(0, 0, 1, 0, 0, 0, 2, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -2283,7 +2292,7 @@
         <v>(0, 1, 0, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -2325,7 +2334,7 @@
         <v>(0, 1, 0, 0, 0, 0, 0, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2367,7 +2376,7 @@
         <v>(0, 1, 0, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -2409,7 +2418,7 @@
         <v>(0, 1, 0, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2451,7 +2460,7 @@
         <v>(0, 1, 0, 0, 0, 0, 1, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2493,7 +2502,7 @@
         <v>(0, 1, 0, 0, 0, 0, 1, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2535,7 +2544,7 @@
         <v>(0, 1, 0, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -2577,7 +2586,7 @@
         <v>(0, 1, 0, 0, 0, 0, 2, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -2619,7 +2628,7 @@
         <v>(0, 1, 0, 0, 0, 0, 2, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -2661,7 +2670,7 @@
         <v>(1, 0, 0, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -2703,7 +2712,7 @@
         <v>(1, 0, 0, 0, 0, 0, 0, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -2745,7 +2754,7 @@
         <v>(1, 0, 0, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -2787,7 +2796,7 @@
         <v>(0, 1, 1, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -2829,7 +2838,7 @@
         <v>(0, 1, 1, 0, 0, 0, 0, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -2871,7 +2880,7 @@
         <v>(0, 1, 1, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -2913,7 +2922,7 @@
         <v>(0, 1, 1, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -2955,7 +2964,7 @@
         <v>(0, 1, 1, 0, 0, 0, 1, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -2997,7 +3006,7 @@
         <v>(0, 1, 1, 0, 0, 0, 1, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -3039,7 +3048,7 @@
         <v>(0, 1, 1, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -3081,7 +3090,7 @@
         <v>(0, 1, 1, 0, 0, 0, 2, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -3123,7 +3132,7 @@
         <v>(0, 1, 1, 0, 0, 0, 2, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -3165,7 +3174,7 @@
         <v>(0, 0, 0, 1, 0, 0, 0, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -3207,7 +3216,7 @@
         <v>(0, 0, 0, 1, 0, 0, 1, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -3249,7 +3258,7 @@
         <v>(0, 0, 0, 1, 0, 0, 2, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -3291,7 +3300,7 @@
         <v>(0, 0, 0, 1, 0, 0, 0, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -3333,7 +3342,7 @@
         <v>(0, 0, 0, 1, 0, 0, 1, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -3375,7 +3384,7 @@
         <v>(0, 0, 0, 1, 0, 0, 2, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -3417,7 +3426,7 @@
         <v>(1, 0, 0, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -3459,7 +3468,7 @@
         <v>(1, 0, 0, 0, 0, 0, 1, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -3501,7 +3510,7 @@
         <v>(1, 0, 0, 0, 0, 0, 1, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -3543,7 +3552,7 @@
         <v>(1, 0, 0, 1, 1, 0, 1, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -3585,7 +3594,7 @@
         <v>(1, 0, 0, 1, 1, 0, 2, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -3627,7 +3636,7 @@
         <v>(1, 1, 1, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -3669,7 +3678,7 @@
         <v>(1, 1, 1, 0, 0, 0, 1, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>71</v>
       </c>
@@ -3711,7 +3720,7 @@
         <v>(1, 1, 1, 0, 0, 0, 1, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -3753,7 +3762,7 @@
         <v>(1, 0, 0, 0, 0, 0, 0, 99, 0, 0)</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>73</v>
       </c>
@@ -3795,7 +3804,7 @@
         <v>(1, 0, 0, 0, 0, 0, 0, 99, 1, 0)</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>74</v>
       </c>
@@ -3837,7 +3846,7 @@
         <v>(1, 0, 0, 0, 0, 0, 0, 99, 2, 0)</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -3879,7 +3888,7 @@
         <v>(1, 1, 1, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>76</v>
       </c>
@@ -3921,7 +3930,7 @@
         <v>(1, 1, 1, 0, 0, 0, 2, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>77</v>
       </c>
@@ -3963,7 +3972,7 @@
         <v>(1, 1, 1, 0, 0, 0, 2, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -4005,7 +4014,7 @@
         <v>(0, 0, 0, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -4047,7 +4056,7 @@
         <v>(0, 0, 0, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>82</v>
       </c>
@@ -4089,7 +4098,7 @@
         <v>(0, 0, 0, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -4131,7 +4140,7 @@
         <v>(0, 0, 0, 0, 0, 0, 0, 2, 0, 0)</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>84</v>
       </c>
@@ -4173,7 +4182,7 @@
         <v>(0, 0, 0, 0, 0, 0, 2, 2, 0, 0)</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -4215,7 +4224,7 @@
         <v>(0, 0, 0, 0, 0, 0, 1, 2, 0, 0)</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -4257,7 +4266,7 @@
         <v>(0, 0, 0, 1, 1, 0, 0, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -4299,7 +4308,7 @@
         <v>(0, 0, 0, 1, 1, 1, 0, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>91</v>
       </c>
@@ -4341,7 +4350,7 @@
         <v>(1, 0, 1, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>86</v>
       </c>
@@ -4383,7 +4392,7 @@
         <v>(1, 0, 1, 0, 0, 0, 1, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>87</v>
       </c>
@@ -4425,7 +4434,7 @@
         <v>(1, 0, 1, 0, 0, 0, 1, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>88</v>
       </c>
@@ -4467,7 +4476,7 @@
         <v>(1, 0, 1, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>89</v>
       </c>
@@ -4509,7 +4518,7 @@
         <v>(1, 0, 1, 0, 0, 0, 2, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>90</v>
       </c>
@@ -4551,7 +4560,7 @@
         <v>(1, 0, 1, 0, 0, 0, 2, 0, 2, 0)</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>92</v>
       </c>
@@ -4589,11 +4598,11 @@
         <v>0</v>
       </c>
       <c r="M81" t="str">
-        <f t="shared" ref="M81:M83" si="5">"("&amp;C81&amp;", "&amp;D81&amp;", "&amp;E81&amp;", "&amp;F81&amp;", "&amp;G81&amp;", "&amp;H81&amp;", "&amp;I81&amp;", "&amp;J81&amp;", "&amp;K81&amp;", "&amp;L81&amp;")"</f>
+        <f t="shared" ref="M81:M86" si="5">"("&amp;C81&amp;", "&amp;D81&amp;", "&amp;E81&amp;", "&amp;F81&amp;", "&amp;G81&amp;", "&amp;H81&amp;", "&amp;I81&amp;", "&amp;J81&amp;", "&amp;K81&amp;", "&amp;L81&amp;")"</f>
         <v>(1, 0, 1, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>93</v>
       </c>
@@ -4635,7 +4644,7 @@
         <v>(1, 0, 1, 0, 0, 0, 0, 0, 1, 0)</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>94</v>
       </c>
@@ -4677,8 +4686,133 @@
         <v>(1, 0, 1, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
     </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>97</v>
+      </c>
+      <c r="B84">
+        <v>26</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84" t="str">
+        <f t="shared" si="5"/>
+        <v>(1, 1, 1, 0, 0, 0, 0, 0, 0, 0)</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>95</v>
+      </c>
+      <c r="B85">
+        <v>26</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>1</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85" t="str">
+        <f t="shared" si="5"/>
+        <v>(1, 1, 1, 0, 0, 0, 0, 0, 1, 0)</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>96</v>
+      </c>
+      <c r="B86">
+        <v>26</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>2</v>
+      </c>
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86" t="str">
+        <f t="shared" si="5"/>
+        <v>(1, 1, 1, 0, 0, 0, 0, 0, 2, 0)</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M80" xr:uid="{1CB244BC-9C72-4B97-907A-D0729174BA0A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added support for ded and min ded
</commit_message>
<xml_diff>
--- a/oasislmf/_data/calc_rules.xlsx
+++ b/oasislmf/_data/calc_rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\OasisLMF\oasislmf\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC09781-1318-404B-957C-995C4E1E58F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627DC94A-08DF-47E1-8802-72C4A3D27E8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>desc</t>
   </si>
@@ -327,6 +327,15 @@
   </si>
   <si>
     <t>deductible with min and max deductible, no limit</t>
+  </si>
+  <si>
+    <t>deductible with min deductible, no limit</t>
+  </si>
+  <si>
+    <t>deductible with min deductible, no limit % loss</t>
+  </si>
+  <si>
+    <t>deductible with min deductible, no limit % TIV</t>
   </si>
 </sst>
 </file>
@@ -1167,13 +1176,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M86"/>
+  <dimension ref="A1:M89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A54" sqref="A54"/>
+      <selection pane="bottomRight" sqref="A1:M89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4812,6 +4821,132 @@
         <v>(1, 1, 1, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
     </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>98</v>
+      </c>
+      <c r="B87">
+        <v>26</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <v>0</v>
+      </c>
+      <c r="M87" t="str">
+        <f t="shared" ref="M87:M89" si="6">"("&amp;C87&amp;", "&amp;D87&amp;", "&amp;E87&amp;", "&amp;F87&amp;", "&amp;G87&amp;", "&amp;H87&amp;", "&amp;I87&amp;", "&amp;J87&amp;", "&amp;K87&amp;", "&amp;L87&amp;")"</f>
+        <v>(1, 1, 0, 0, 0, 0, 0, 0, 0, 0)</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>99</v>
+      </c>
+      <c r="B88">
+        <v>26</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+      <c r="K88">
+        <v>1</v>
+      </c>
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88" t="str">
+        <f t="shared" si="6"/>
+        <v>(1, 1, 0, 0, 0, 0, 0, 0, 1, 0)</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>100</v>
+      </c>
+      <c r="B89">
+        <v>26</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>2</v>
+      </c>
+      <c r="L89">
+        <v>0</v>
+      </c>
+      <c r="M89" t="str">
+        <f t="shared" si="6"/>
+        <v>(1, 1, 0, 0, 0, 0, 0, 0, 2, 0)</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>